<commit_message>
Backup graph scripts and experiments
</commit_message>
<xml_diff>
--- a/graphs/delay_aware_slicing/average_results/average_results.xlsx
+++ b/graphs/delay_aware_slicing/average_results/average_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phisolani/Github/wifi_monitoring/graphs/delay_aware_slicing/average_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AFE6EC-33D4-5449-A7E4-5BD6CF6C06E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212AAD44-63C4-A14D-A520-6A636A8ED2CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20700" yWindow="500" windowWidth="17700" windowHeight="18820" xr2:uid="{3FEC7344-D201-3244-A186-2559A3F9F96E}"/>
   </bookViews>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70784E4A-0428-264E-82D8-1E226FAD8D1C}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,15 +1533,15 @@
         <v>339.84319038673863</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37" si="18">AVERAGE(D27:D36)</f>
+        <f t="shared" ref="D37:E37" si="18">AVERAGE(D27:D36)</f>
         <v>386.18693064093236</v>
       </c>
       <c r="E37">
-        <f t="shared" ref="E37" si="19">AVERAGE(E27:E36)</f>
+        <f t="shared" si="18"/>
         <v>240.21090278599576</v>
       </c>
       <c r="F37">
-        <f t="shared" ref="F37" si="20">AVERAGE(F27:F36)</f>
+        <f t="shared" ref="F37" si="19">AVERAGE(F27:F36)</f>
         <v>179.69304080674812</v>
       </c>
       <c r="H37" t="s">
@@ -1552,19 +1552,19 @@
         <v>32.082469153854873</v>
       </c>
       <c r="J37">
-        <f t="shared" ref="J37" si="21">AVERAGE(J27:J36)</f>
+        <f t="shared" ref="J37" si="20">AVERAGE(J27:J36)</f>
         <v>374.27179474129753</v>
       </c>
       <c r="K37">
-        <f t="shared" ref="K37" si="22">AVERAGE(K27:K36)</f>
+        <f t="shared" ref="K37" si="21">AVERAGE(K27:K36)</f>
         <v>428.42693071549667</v>
       </c>
       <c r="L37">
-        <f t="shared" ref="L37" si="23">AVERAGE(L27:L36)</f>
+        <f t="shared" ref="L37" si="22">AVERAGE(L27:L36)</f>
         <v>407.40703879961779</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M37" si="24">AVERAGE(M27:M36)</f>
+        <f t="shared" ref="M37" si="23">AVERAGE(M27:M36)</f>
         <v>96.548140369173311</v>
       </c>
     </row>
@@ -1577,19 +1577,19 @@
         <v>14.920146233959088</v>
       </c>
       <c r="C38">
-        <f t="shared" ref="C38:F38" si="25">STDEV(C27:C36)</f>
+        <f t="shared" ref="C38:F38" si="24">STDEV(C27:C36)</f>
         <v>45.557866369419351</v>
       </c>
       <c r="D38">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>52.37109333155329</v>
       </c>
       <c r="E38">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>92.142601107525238</v>
       </c>
       <c r="F38">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>29.790279390320507</v>
       </c>
       <c r="H38" t="s">
@@ -1600,19 +1600,19 @@
         <v>9.3920629556874804</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:M38" si="26">STDEV(J27:J36)</f>
+        <f t="shared" ref="J38:M38" si="25">STDEV(J27:J36)</f>
         <v>35.370213728769542</v>
       </c>
       <c r="K38">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>37.682792833618386</v>
       </c>
       <c r="L38">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>78.798406394632963</v>
       </c>
       <c r="M38">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>28.48412061182173</v>
       </c>
     </row>
@@ -1625,19 +1625,19 @@
         <v>4.7181645122094196</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39" si="27">C38/(SQRT(10))</f>
+        <f t="shared" ref="C39" si="26">C38/(SQRT(10))</f>
         <v>14.406662306495111</v>
       </c>
       <c r="D39">
-        <f t="shared" ref="D39" si="28">D38/(SQRT(10))</f>
+        <f t="shared" ref="D39" si="27">D38/(SQRT(10))</f>
         <v>16.561193848096416</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39" si="29">E38/(SQRT(10))</f>
+        <f t="shared" ref="E39" si="28">E38/(SQRT(10))</f>
         <v>29.138048903213321</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="F39" si="30">F38/(SQRT(10))</f>
+        <f t="shared" ref="F39" si="29">F38/(SQRT(10))</f>
         <v>9.4205135006185028</v>
       </c>
       <c r="H39" t="s">
@@ -1648,19 +1648,19 @@
         <v>2.9700310867665518</v>
       </c>
       <c r="J39">
-        <f t="shared" ref="J39" si="31">J38/(SQRT(10))</f>
+        <f t="shared" ref="J39" si="30">J38/(SQRT(10))</f>
         <v>11.185043670986882</v>
       </c>
       <c r="K39">
-        <f t="shared" ref="K39" si="32">K38/(SQRT(10))</f>
+        <f t="shared" ref="K39" si="31">K38/(SQRT(10))</f>
         <v>11.916345395050451</v>
       </c>
       <c r="L39">
-        <f t="shared" ref="L39" si="33">L38/(SQRT(10))</f>
+        <f t="shared" ref="L39" si="32">L38/(SQRT(10))</f>
         <v>24.918244019861696</v>
       </c>
       <c r="M39">
-        <f t="shared" ref="M39" si="34">M38/(SQRT(10))</f>
+        <f t="shared" ref="M39" si="33">M38/(SQRT(10))</f>
         <v>9.0074698280305512</v>
       </c>
     </row>
@@ -1673,19 +1673,19 @@
         <v>9.4363290244188391</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40" si="35">2*C39</f>
+        <f t="shared" ref="C40" si="34">2*C39</f>
         <v>28.813324612990222</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40" si="36">2*D39</f>
+        <f t="shared" ref="D40" si="35">2*D39</f>
         <v>33.122387696192831</v>
       </c>
       <c r="E40">
-        <f t="shared" ref="E40" si="37">2*E39</f>
+        <f t="shared" ref="E40" si="36">2*E39</f>
         <v>58.276097806426641</v>
       </c>
       <c r="F40">
-        <f t="shared" ref="F40" si="38">2*F39</f>
+        <f t="shared" ref="F40" si="37">2*F39</f>
         <v>18.841027001237006</v>
       </c>
       <c r="H40" t="s">
@@ -1696,19 +1696,19 @@
         <v>5.9400621735331036</v>
       </c>
       <c r="J40">
-        <f t="shared" ref="J40" si="39">2*J39</f>
+        <f t="shared" ref="J40" si="38">2*J39</f>
         <v>22.370087341973765</v>
       </c>
       <c r="K40">
-        <f t="shared" ref="K40" si="40">2*K39</f>
+        <f t="shared" ref="K40" si="39">2*K39</f>
         <v>23.832690790100902</v>
       </c>
       <c r="L40">
-        <f t="shared" ref="L40" si="41">2*L39</f>
+        <f t="shared" ref="L40" si="40">2*L39</f>
         <v>49.836488039723392</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40" si="42">2*M39</f>
+        <f t="shared" ref="M40" si="41">2*M39</f>
         <v>18.014939656061102</v>
       </c>
     </row>

</xml_diff>